<commit_message>
T1135_T1136_Contacts_CampaignHistory_AddToCampaign_SaveCancelEditUpdate - Mid - 22 Oct 2024
</commit_message>
<xml_diff>
--- a/TestData/T1135_T1136_Contacts_CampaignHistory_AddToCampaign_SaveCancelEditUpdate.xlsx
+++ b/TestData/T1135_T1136_Contacts_CampaignHistory_AddToCampaign_SaveCancelEditUpdate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77CB678-E4AE-4D57-AB0B-377184D28C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5388BE3A-A907-4607-BFAF-1FEC62BAFE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,9 +496,9 @@
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="12.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -513,13 +513,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -536,13 +536,13 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -550,7 +550,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{0D7A005D-A1B3-4C06-A618-E275ADEF2E12}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{0D7A005D-A1B3-4C06-A618-E275ADEF2E12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
Contacts - 23 April
</commit_message>
<xml_diff>
--- a/TestData/T1135_T1136_Contacts_CampaignHistory_AddToCampaign_SaveCancelEditUpdate.xlsx
+++ b/TestData/T1135_T1136_Contacts_CampaignHistory_AddToCampaign_SaveCancelEditUpdate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5388BE3A-A907-4607-BFAF-1FEC62BAFE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C789D2-DFD4-4D3B-B6E4-430372BC2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>HL Sub Group</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>BUS</t>
   </si>
   <si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>Ayati Arvind</t>
+  </si>
+  <si>
+    <t>BAS</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -513,36 +513,36 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,13 +628,13 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -659,21 +659,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Contacts CHanges - Mid - 18 June 2025
</commit_message>
<xml_diff>
--- a/TestData/T1135_T1136_Contacts_CampaignHistory_AddToCampaign_SaveCancelEditUpdate.xlsx
+++ b/TestData/T1135_T1136_Contacts_CampaignHistory_AddToCampaign_SaveCancelEditUpdate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C789D2-DFD4-4D3B-B6E4-430372BC2E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685D0762-377F-4C30-83E5-620BBE08F321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="1500" windowWidth="19416" windowHeight="10740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
     <t>Ayati Arvind</t>
   </si>
   <si>
-    <t>BAS</t>
+    <t>None</t>
   </si>
 </sst>
 </file>

</xml_diff>